<commit_message>
Update frontend and backend with latest changes
</commit_message>
<xml_diff>
--- a/backend/registrations.xlsx
+++ b/backend/registrations.xlsx
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -440,9 +440,56 @@
         <v>Registration Date</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>kjnkjnnj</v>
+      </c>
+      <c r="B2" t="str">
+        <v>sefegf</v>
+      </c>
+      <c r="C2" t="str">
+        <v>gfegfe</v>
+      </c>
+      <c r="D2" t="str">
+        <v>gfegfeg</v>
+      </c>
+      <c r="E2" t="str">
+        <v>aditya@gmail.com</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Duo</v>
+      </c>
+      <c r="G2" t="str">
+        <v>sfwe</v>
+      </c>
+      <c r="H2" t="str">
+        <v>2</v>
+      </c>
+      <c r="I2" t="str">
+        <v>true</v>
+      </c>
+      <c r="J2" t="str">
+        <v>GPay</v>
+      </c>
+      <c r="K2" t="str">
+        <v>8018389108</v>
+      </c>
+      <c r="L2" t="str">
+        <v>1769031913866-Gemini_Generated_Image_gmm0m4gmm0m4gmm0.png</v>
+      </c>
+      <c r="M2" t="str">
+        <v>true</v>
+      </c>
+      <c r="N2" t="str">
+        <v>true</v>
+      </c>
+      <c r="O2" t="str">
+        <v>22/01/2026, 03:15:14</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>